<commit_message>
210222 更新，針對 210208 更新文件 (PPT)
</commit_message>
<xml_diff>
--- a/demo-images/_頁面清單.xlsx
+++ b/demo-images/_頁面清單.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ladies-inlove.com\demo-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B335F94C-6B56-403B-BC4F-1094AEF487A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB78FD1D-865F-418D-B943-5041C8D3811C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
   <si>
     <t>頁面名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,207 +275,233 @@
     <t>integral.html</t>
   </si>
   <si>
+    <t>bid-list1.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>products.html</t>
+  </si>
+  <si>
+    <t>products-detail.html</t>
+  </si>
+  <si>
+    <t>products-list1.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>products-list2.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-result-none.html</t>
+  </si>
+  <si>
+    <t>search-result.html</t>
+  </si>
+  <si>
+    <t>member-post.html</t>
+  </si>
+  <si>
+    <t>seller-order.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-products-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-data.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-program.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-product.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-products.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-posts.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-evaluation.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-blog.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-options.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-data-security.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-order-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-order-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-order.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-reward.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-realname-1.html</t>
+  </si>
+  <si>
+    <t>member-realname-2-finish.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實名認證</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-realname-2.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實名認證-手機信箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-realname-3.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實名認證-傳資料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-realname-4.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-realname-5.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實名認證-等待</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實名認證-完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integral-list1.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-data-pay.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-data-address.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blog-detail.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vip.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-favorites1.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文章列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-post-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忘記密碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login-forget.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login-reset.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重設密碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>填寫會員註冊資料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login-register.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>integral-detail.html</t>
-  </si>
-  <si>
-    <t>bid-list1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>products.html</t>
-  </si>
-  <si>
-    <t>products-detail.html</t>
-  </si>
-  <si>
-    <t>products-list1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>products-list2.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>index.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search-result-none.html</t>
-  </si>
-  <si>
-    <t>search-result.html</t>
-  </si>
-  <si>
-    <t>member-post.html</t>
-  </si>
-  <si>
-    <t>seller-order.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seller-products-list.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-data.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seller-program.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seller-product.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop-products.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop-posts.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop-evaluation.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop-blog.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seller-options.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-data-security.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seller-order-list.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-order-list.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-order.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-reward.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>member-identification.html</t>
-  </si>
-  <si>
-    <t>member-realname-1.html</t>
-  </si>
-  <si>
-    <t>member-realname-2-finish.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實名認證</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-realname-2.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實名認證-手機信箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-realname-3.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實名認證-傳資料</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-realname-4.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-realname-5.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實名認證-等待</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>實名認證-完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>integral-list1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-data-pay.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-data-address.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>blog-detail.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vip.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-favorites1.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文章列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>member-post-list.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>忘記密碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login-forget.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login-reset.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重設密碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>填寫會員註冊資料</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login-register.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鑑定紀錄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member-identification-log.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>購買刊登筆數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-service.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>購買 VIP 會員方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seller-service-checkout.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -829,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -860,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -871,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -879,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -887,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -895,7 +921,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -914,7 +940,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -949,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -957,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -965,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -976,7 +1002,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -984,7 +1010,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -995,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1003,7 +1029,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1011,7 +1037,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1019,7 +1045,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1027,7 +1053,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1081,7 +1107,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1127,31 +1153,31 @@
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1159,7 +1185,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1175,7 +1201,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1183,7 +1209,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1194,7 +1220,7 @@
         <v>37</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1202,7 +1228,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1210,7 +1236,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1218,7 +1244,7 @@
         <v>40</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1226,7 +1252,7 @@
         <v>45</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1237,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1245,55 +1271,55 @@
         <v>33</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="C49" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>91</v>
@@ -1301,66 +1327,90 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>77</v>
+      <c r="C61" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>